<commit_message>
we will need a bigger boat
</commit_message>
<xml_diff>
--- a/chikito.xlsx
+++ b/chikito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\VNTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFA1414-50FA-4507-B75E-9490B227B613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9C6D80-3747-404B-B3D9-97B0505159EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
creating recursivity by performance
</commit_message>
<xml_diff>
--- a/chikito.xlsx
+++ b/chikito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\VNTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9C6D80-3747-404B-B3D9-97B0505159EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA19A6E-BCBF-4E3E-8322-3641D7A214FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD15"/>
+      <selection activeCell="A18" sqref="A18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1174,34 +1174,10 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
     <row r="9" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="14"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1355,13 +1331,12 @@
       <c r="J21" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C18:C19"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adding logic depending of the decision type
</commit_message>
<xml_diff>
--- a/chikito.xlsx
+++ b/chikito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\VNTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA19A6E-BCBF-4E3E-8322-3641D7A214FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288B769E-C2BA-4A03-9FFA-35EDD7AC12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Con Liz'Amar solos en la habitación de Berto</t>
+  </si>
+  <si>
+    <t>Pasar el rato con ella</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Salir a entrenar</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>4,-1</t>
   </si>
 </sst>
 </file>
@@ -628,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,6 +697,12 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1032,7 +1062,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1174,6 +1204,50 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
+    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="9" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
@@ -1331,12 +1405,13 @@
       <c r="J21" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>